<commit_message>
xgb threshold tuning and payoff matrix
</commit_message>
<xml_diff>
--- a/references/GoTyme interview case study.xlsx
+++ b/references/GoTyme interview case study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Interviews\Case Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JV\Documents\Case Studies\GoTyme\gt_propensity_model\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BDE9BB-A556-4931-88B7-DDB6D6FBBB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08D14B5-B54A-4C81-9357-6DB055E26F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2B46F2EB-801E-42E1-9486-C5F4ABA8029D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2B46F2EB-801E-42E1-9486-C5F4ABA8029D}"/>
   </bookViews>
   <sheets>
     <sheet name="Case study" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="102">
   <si>
     <t>Variable</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t xml:space="preserve">and they have classified the customers accordingly into the following 3 risk bands  </t>
+  </si>
+  <si>
+    <t>Person A</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t>Payoffs</t>
   </si>
 </sst>
 </file>
@@ -379,9 +391,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -390,11 +403,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,9 +424,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -450,7 +464,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -556,7 +570,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -698,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -706,237 +720,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C5458A-C9EB-483D-A5EC-49E4759AD2B0}">
-  <dimension ref="B3:F64"/>
+  <dimension ref="B3:K103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="S90" sqref="S90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" s="6" t="s">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" s="6" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" s="6" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" s="6" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="4"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="6" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="5"/>
       <c r="D50" s="3" t="s">
         <v>83</v>
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
       <c r="C51" t="s">
         <v>55</v>
@@ -946,7 +960,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
       <c r="C52" t="s">
         <v>56</v>
@@ -956,7 +970,7 @@
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
       <c r="C53" t="s">
         <v>57</v>
@@ -966,15 +980,15 @@
       </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
       <c r="D56" s="3" t="s">
         <v>94</v>
@@ -983,7 +997,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="4"/>
       <c r="C57" t="s">
         <v>55</v>
@@ -995,7 +1009,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="4"/>
       <c r="C58" t="s">
         <v>56</v>
@@ -1007,7 +1021,7 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
       <c r="C59" t="s">
         <v>57</v>
@@ -1019,26 +1033,373 @@
         <v>-300</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68">
+        <v>0.1</v>
+      </c>
+      <c r="F68">
+        <v>0.25</v>
+      </c>
+      <c r="G68">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>5553</v>
+      </c>
+      <c r="E72">
+        <v>659</v>
+      </c>
+      <c r="G72">
+        <f>SUM(D72:E73)</f>
+        <v>6998</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>137</v>
+      </c>
+      <c r="E73">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" s="6">
+        <f>D72/$G$72</f>
+        <v>0.7935124321234639</v>
+      </c>
+      <c r="E76" s="6">
+        <f t="shared" ref="E76:E77" si="0">E72/$G$72</f>
+        <v>9.4169762789368394E-2</v>
+      </c>
+      <c r="H76" t="s">
+        <v>101</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>300</v>
+      </c>
+      <c r="K76">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" s="6">
+        <f t="shared" ref="D77" si="1">D73/$G$72</f>
+        <v>1.9577022006287512E-2</v>
+      </c>
+      <c r="E77" s="6">
+        <f t="shared" si="0"/>
+        <v>9.2740783080880254E-2</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <f>0.1*-285 + 0.25*-705 + 0.65*-1225</f>
+        <v>-1001</v>
+      </c>
+      <c r="K77">
+        <f>0.1*285 + 0.25*705 + 0.65*1225</f>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <f>D76*J76+D77*J77+E76*K76+E77*K77</f>
+        <v>283.03972563589599</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>24848</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <f>SUM(D84:E85)</f>
+        <v>27991</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>3143</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" s="6">
+        <f>D84/$G$84</f>
+        <v>0.88771390804187056</v>
+      </c>
+      <c r="E88" s="6">
+        <f t="shared" ref="E88:E89" si="2">E84/$G$84</f>
+        <v>0</v>
+      </c>
+      <c r="H88" t="s">
+        <v>101</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>300</v>
+      </c>
+      <c r="K88">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89" s="6">
+        <f t="shared" ref="D89" si="3">D85/$G$84</f>
+        <v>0.1122860919581294</v>
+      </c>
+      <c r="E89" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <f>0.1*-285 + 0.25*-705 + 0.65*-1225</f>
+        <v>-1001</v>
+      </c>
+      <c r="K89">
+        <f>0.1*285 + 0.25*705 + 0.65*1225</f>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <f>D88*J88+D89*J89+E88*K88+E89*K89</f>
+        <v>153.91579436247363</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E94" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>24848</v>
+      </c>
+      <c r="G96">
+        <f>SUM(D96:E97)</f>
+        <v>27991</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" s="6">
+        <f>D96/$G$96</f>
+        <v>0</v>
+      </c>
+      <c r="E100" s="6">
+        <f t="shared" ref="E100:E101" si="4">E96/$G$96</f>
+        <v>0.88771390804187056</v>
+      </c>
+      <c r="H100" t="s">
+        <v>101</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>300</v>
+      </c>
+      <c r="K100">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" s="6">
+        <f t="shared" ref="D101" si="5">D97/$G$96</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="6">
+        <f t="shared" si="4"/>
+        <v>0.1122860919581294</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <f>0.1*-285 + 0.25*-705 + 0.65*-1225</f>
+        <v>-1001</v>
+      </c>
+      <c r="K101">
+        <f>0.1*285 + 0.25*705 + 0.65*1225</f>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <f>D100*J100+D101*J101+E100*K100+E101*K101</f>
+        <v>-153.91579436247363</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1051,17 +1412,17 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="96.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="96.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1083,7 +1444,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -1094,7 +1455,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1105,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1116,7 +1477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1127,7 +1488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1138,7 +1499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1149,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1160,7 +1521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1171,7 +1532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1182,7 +1543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1193,7 +1554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1204,7 +1565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1215,7 +1576,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1226,7 +1587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -1237,7 +1598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1248,7 +1609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -1259,7 +1620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1270,7 +1631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1281,7 +1642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1292,7 +1653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>

</xml_diff>